<commit_message>
Revert "matlab for plotting"
This reverts commit c7724c656db40cdae4a9ffac2f12cc1cd845a14b
</commit_message>
<xml_diff>
--- a/data_pi/bcode/perf_data_backup/runtime_results_for_graph.xlsx
+++ b/data_pi/bcode/perf_data_backup/runtime_results_for_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>average</t>
   </si>
@@ -54,16 +54,13 @@
   <si>
     <t>clock ticks in seconds</t>
   </si>
-  <si>
-    <t>PC</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -132,7 +129,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,12 +425,12 @@
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -443,12 +440,9 @@
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>24</v>
       </c>
@@ -461,11 +455,8 @@
         <f>C4/A4</f>
         <v>1.0096375</v>
       </c>
-      <c r="H4" s="1">
-        <v>4.4687700000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>18</v>
       </c>
@@ -478,11 +469,8 @@
         <f t="shared" ref="E5:E36" si="0">C5/A5</f>
         <v>1.052861111111111</v>
       </c>
-      <c r="H5" s="1">
-        <v>3.5154000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>69</v>
       </c>
@@ -495,11 +483,8 @@
         <f t="shared" si="0"/>
         <v>1.0305623188405797</v>
       </c>
-      <c r="H6" s="1">
-        <v>13.2567</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36</v>
       </c>
@@ -512,11 +497,8 @@
         <f t="shared" si="0"/>
         <v>1.0061388888888887</v>
       </c>
-      <c r="H7" s="1">
-        <v>6.8480299999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>15</v>
       </c>
@@ -527,11 +509,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="1">
-        <v>2.88348</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>24</v>
       </c>
@@ -544,11 +523,8 @@
         <f t="shared" si="0"/>
         <v>1.0464374999999999</v>
       </c>
-      <c r="H9" s="1">
-        <v>4.74308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>21</v>
       </c>
@@ -561,11 +537,8 @@
         <f t="shared" si="0"/>
         <v>1.0145333333333333</v>
       </c>
-      <c r="H10" s="1">
-        <v>4.0417399999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>27</v>
       </c>
@@ -578,11 +551,8 @@
         <f t="shared" si="0"/>
         <v>1.0504888888888888</v>
       </c>
-      <c r="H11" s="1">
-        <v>5.33439</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>258</v>
       </c>
@@ -593,11 +563,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="1">
-        <v>49.197899999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>114</v>
       </c>
@@ -610,11 +577,8 @@
         <f t="shared" si="0"/>
         <v>1.0503157894736843</v>
       </c>
-      <c r="H13" s="1">
-        <v>22.186599999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -627,11 +591,8 @@
         <f t="shared" si="0"/>
         <v>1.0379761904761904</v>
       </c>
-      <c r="H14" s="1">
-        <v>8.2570800000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>57</v>
       </c>
@@ -644,11 +605,8 @@
         <f t="shared" si="0"/>
         <v>1.0612368421052631</v>
       </c>
-      <c r="H15" s="1">
-        <v>11.2111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>24</v>
       </c>
@@ -661,11 +619,8 @@
         <f t="shared" si="0"/>
         <v>1.0368416666666667</v>
       </c>
-      <c r="H16" s="1">
-        <v>4.5270299999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>27</v>
       </c>
@@ -678,11 +633,8 @@
         <f t="shared" si="0"/>
         <v>1.0145629629629629</v>
       </c>
-      <c r="H17" s="1">
-        <v>5.11944</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -693,11 +645,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="1">
-        <v>2.9321799999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -710,11 +659,8 @@
         <f t="shared" si="0"/>
         <v>1.0434177777777778</v>
       </c>
-      <c r="H19" s="1">
-        <v>8.7858900000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -725,11 +671,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="1">
-        <v>2.8101799999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -742,11 +685,8 @@
         <f t="shared" si="0"/>
         <v>1.0174476190476189</v>
       </c>
-      <c r="H21" s="1">
-        <v>3.9437799999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>27</v>
       </c>
@@ -759,11 +699,8 @@
         <f t="shared" si="0"/>
         <v>1.0475925925925926</v>
       </c>
-      <c r="H22" s="1">
-        <v>5.3283800000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>51</v>
       </c>
@@ -776,11 +713,8 @@
         <f t="shared" si="0"/>
         <v>1.0536392156862744</v>
       </c>
-      <c r="H23" s="1">
-        <v>10.084899999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>84</v>
       </c>
@@ -793,11 +727,8 @@
         <f t="shared" si="0"/>
         <v>1.0331785714285715</v>
       </c>
-      <c r="H24" s="1">
-        <v>16.335599999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>27</v>
       </c>
@@ -810,11 +741,8 @@
         <f t="shared" si="0"/>
         <v>1.0538888888888889</v>
       </c>
-      <c r="H25" s="1">
-        <v>5.2711100000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45</v>
       </c>
@@ -827,11 +755,8 @@
         <f t="shared" si="0"/>
         <v>1.0544755555555556</v>
       </c>
-      <c r="H26" s="1">
-        <v>8.8572799999999994</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>36</v>
       </c>
@@ -844,11 +769,8 @@
         <f t="shared" si="0"/>
         <v>1.0373138888888889</v>
       </c>
-      <c r="H27" s="1">
-        <v>6.9883199999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>39</v>
       </c>
@@ -861,11 +783,8 @@
         <f t="shared" si="0"/>
         <v>1.0201461538461538</v>
       </c>
-      <c r="H28" s="1">
-        <v>7.6944999999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>33</v>
       </c>
@@ -878,11 +797,8 @@
         <f t="shared" si="0"/>
         <v>1.0116424242424242</v>
       </c>
-      <c r="H29" s="1">
-        <v>6.2503099999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -895,11 +811,8 @@
         <f t="shared" si="0"/>
         <v>1.0222074074074075</v>
       </c>
-      <c r="H30" s="1">
-        <v>5.1136799999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>72</v>
       </c>
@@ -912,11 +825,8 @@
         <f t="shared" si="0"/>
         <v>1.0457444444444444</v>
       </c>
-      <c r="H31" s="1">
-        <v>14.0959</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>72</v>
       </c>
@@ -929,11 +839,8 @@
         <f t="shared" si="0"/>
         <v>1.0364250000000002</v>
       </c>
-      <c r="H32" s="1">
-        <v>13.969900000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>21</v>
       </c>
@@ -946,11 +853,8 @@
         <f t="shared" si="0"/>
         <v>1.0145952380952381</v>
       </c>
-      <c r="H33" s="1">
-        <v>4.0094099999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>72</v>
       </c>
@@ -963,11 +867,8 @@
         <f t="shared" si="0"/>
         <v>1.0685041666666666</v>
       </c>
-      <c r="H34" s="1">
-        <v>14.328200000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>126</v>
       </c>
@@ -978,11 +879,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H35" s="1">
-        <v>24.922999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>51</v>
       </c>
@@ -995,17 +893,14 @@
         <f t="shared" si="0"/>
         <v>1.0341392156862745</v>
       </c>
-      <c r="H36" s="1">
-        <v>9.92666</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1017,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1031,55 +926,55 @@
         <v>0.37176417224093994</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1173,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "do it again"
This reverts commit 80fcf50c83f3ea39cf50e79a867d759fc36038ab
</commit_message>
<xml_diff>
--- a/data_pi/bcode/perf_data_backup/runtime_results_for_graph.xlsx
+++ b/data_pi/bcode/perf_data_backup/runtime_results_for_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>average</t>
   </si>
@@ -54,16 +54,13 @@
   <si>
     <t>clock ticks in seconds</t>
   </si>
-  <si>
-    <t>PC</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -132,7 +129,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,12 +425,12 @@
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -443,12 +440,9 @@
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>24</v>
       </c>
@@ -461,19 +455,8 @@
         <f>C4/A4</f>
         <v>1.0096375</v>
       </c>
-      <c r="H4" s="1">
-        <v>4.4687700000000001</v>
-      </c>
-      <c r="J4">
-        <f>C4/H4</f>
-        <v>5.4223645432635825</v>
-      </c>
-      <c r="L4">
-        <f>H4/A4</f>
-        <v>0.18619875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>18</v>
       </c>
@@ -486,19 +469,8 @@
         <f t="shared" ref="E5:E36" si="0">C5/A5</f>
         <v>1.052861111111111</v>
       </c>
-      <c r="H5" s="1">
-        <v>3.5154000000000001</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J36" si="1">C5/H5</f>
-        <v>5.3909939124992885</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L36" si="2">H5/A5</f>
-        <v>0.1953</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>69</v>
       </c>
@@ -511,19 +483,8 @@
         <f t="shared" si="0"/>
         <v>1.0305623188405797</v>
       </c>
-      <c r="H6" s="1">
-        <v>13.2567</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>5.3639895298226561</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>0.19212608695652175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36</v>
       </c>
@@ -536,39 +497,20 @@
         <f t="shared" si="0"/>
         <v>1.0061388888888887</v>
       </c>
-      <c r="H7" s="1">
-        <v>6.8480299999999996</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
-        <v>5.2892583706555021</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>0.19022305555555555</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>15</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="H8" s="1">
-        <v>2.88348</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>0.19223200000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>24</v>
       </c>
@@ -581,19 +523,8 @@
         <f t="shared" si="0"/>
         <v>1.0464374999999999</v>
       </c>
-      <c r="H9" s="1">
-        <v>4.74308</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>5.2949771034854987</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0.19762833333333332</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>21</v>
       </c>
@@ -606,19 +537,8 @@
         <f t="shared" si="0"/>
         <v>1.0145333333333333</v>
       </c>
-      <c r="H10" s="1">
-        <v>4.0417399999999999</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>5.2712940466234839</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>0.19246380952380951</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>27</v>
       </c>
@@ -631,39 +551,20 @@
         <f t="shared" si="0"/>
         <v>1.0504888888888888</v>
       </c>
-      <c r="H11" s="1">
-        <v>5.33439</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
-        <v>5.3170465601502697</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0.19757</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>258</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="H12" s="1">
-        <v>49.197899999999997</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="1"/>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0.19068953488372092</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>114</v>
       </c>
@@ -676,19 +577,8 @@
         <f t="shared" si="0"/>
         <v>1.0503157894736843</v>
       </c>
-      <c r="H13" s="1">
-        <v>22.186599999999999</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>5.3967710239513949</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
-        <v>0.19461929824561403</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -701,19 +591,8 @@
         <f t="shared" si="0"/>
         <v>1.0379761904761904</v>
       </c>
-      <c r="H14" s="1">
-        <v>8.2570800000000002</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>5.2797114718520346</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
-        <v>0.19659714285714286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>57</v>
       </c>
@@ -726,19 +605,8 @@
         <f t="shared" si="0"/>
         <v>1.0612368421052631</v>
       </c>
-      <c r="H15" s="1">
-        <v>11.2111</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
-        <v>5.3955900848266447</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>0.19668596491228071</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>24</v>
       </c>
@@ -751,19 +619,8 @@
         <f t="shared" si="0"/>
         <v>1.0368416666666667</v>
       </c>
-      <c r="H16" s="1">
-        <v>4.5270299999999999</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>5.4968047483670306</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
-        <v>0.18862625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>27</v>
       </c>
@@ -776,39 +633,20 @@
         <f t="shared" si="0"/>
         <v>1.0145629629629629</v>
       </c>
-      <c r="H17" s="1">
-        <v>5.11944</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
-        <v>5.3508196208960355</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>0.18960888888888888</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="H18" s="1">
-        <v>2.9321799999999998</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="1"/>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>0.19547866666666666</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -821,39 +659,20 @@
         <f t="shared" si="0"/>
         <v>1.0434177777777778</v>
       </c>
-      <c r="H19" s="1">
-        <v>8.7858900000000002</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
-        <v>5.3442280747880977</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="2"/>
-        <v>0.195242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="H20" s="1">
-        <v>2.8101799999999999</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="2"/>
-        <v>0.18734533333333334</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -866,19 +685,8 @@
         <f t="shared" si="0"/>
         <v>1.0174476190476189</v>
       </c>
-      <c r="H21" s="1">
-        <v>3.9437799999999998</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="1"/>
-        <v>5.4177464260176782</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>0.18779904761904762</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>27</v>
       </c>
@@ -891,19 +699,8 @@
         <f t="shared" si="0"/>
         <v>1.0475925925925926</v>
       </c>
-      <c r="H22" s="1">
-        <v>5.3283800000000001</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="1"/>
-        <v>5.3083676464516421</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="2"/>
-        <v>0.19734740740740742</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>51</v>
       </c>
@@ -916,19 +713,8 @@
         <f t="shared" si="0"/>
         <v>1.0536392156862744</v>
       </c>
-      <c r="H23" s="1">
-        <v>10.084899999999999</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
-        <v>5.3283225416216329</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="2"/>
-        <v>0.19774313725490195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>84</v>
       </c>
@@ -941,19 +727,8 @@
         <f t="shared" si="0"/>
         <v>1.0331785714285715</v>
       </c>
-      <c r="H24" s="1">
-        <v>16.335599999999999</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="1"/>
-        <v>5.3127525159773752</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="2"/>
-        <v>0.19447142857142857</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>27</v>
       </c>
@@ -966,19 +741,8 @@
         <f t="shared" si="0"/>
         <v>1.0538888888888889</v>
       </c>
-      <c r="H25" s="1">
-        <v>5.2711100000000002</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="1"/>
-        <v>5.3982937180214412</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="2"/>
-        <v>0.19522629629629631</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45</v>
       </c>
@@ -991,19 +755,8 @@
         <f t="shared" si="0"/>
         <v>1.0544755555555556</v>
       </c>
-      <c r="H26" s="1">
-        <v>8.8572799999999994</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="1"/>
-        <v>5.3573331767766179</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="2"/>
-        <v>0.19682844444444442</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>36</v>
       </c>
@@ -1016,19 +769,8 @@
         <f t="shared" si="0"/>
         <v>1.0373138888888889</v>
       </c>
-      <c r="H27" s="1">
-        <v>6.9883199999999999</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="1"/>
-        <v>5.343673443688898</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="2"/>
-        <v>0.19411999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>39</v>
       </c>
@@ -1041,19 +783,8 @@
         <f t="shared" si="0"/>
         <v>1.0201461538461538</v>
       </c>
-      <c r="H28" s="1">
-        <v>7.6944999999999997</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
-        <v>5.1706673598024562</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="2"/>
-        <v>0.19729487179487179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>33</v>
       </c>
@@ -1066,19 +797,8 @@
         <f t="shared" si="0"/>
         <v>1.0116424242424242</v>
       </c>
-      <c r="H29" s="1">
-        <v>6.2503099999999998</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="1"/>
-        <v>5.3412070761290238</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="2"/>
-        <v>0.18940333333333334</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1091,19 +811,8 @@
         <f t="shared" si="0"/>
         <v>1.0222074074074075</v>
       </c>
-      <c r="H30" s="1">
-        <v>5.1136799999999996</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="1"/>
-        <v>5.3972090549271758</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="2"/>
-        <v>0.18939555555555554</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>72</v>
       </c>
@@ -1116,19 +825,8 @@
         <f t="shared" si="0"/>
         <v>1.0457444444444444</v>
       </c>
-      <c r="H31" s="1">
-        <v>14.0959</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="1"/>
-        <v>5.3415248405564739</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="2"/>
-        <v>0.1957763888888889</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>72</v>
       </c>
@@ -1141,19 +839,8 @@
         <f t="shared" si="0"/>
         <v>1.0364250000000002</v>
       </c>
-      <c r="H32" s="1">
-        <v>13.969900000000001</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>5.3416703054424159</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="2"/>
-        <v>0.1940263888888889</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>21</v>
       </c>
@@ -1166,19 +853,8 @@
         <f t="shared" si="0"/>
         <v>1.0145952380952381</v>
       </c>
-      <c r="H33" s="1">
-        <v>4.0094099999999999</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="1"/>
-        <v>5.3141235244088278</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="2"/>
-        <v>0.19092428571428571</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>72</v>
       </c>
@@ -1191,39 +867,20 @@
         <f t="shared" si="0"/>
         <v>1.0685041666666666</v>
       </c>
-      <c r="H34" s="1">
-        <v>14.328200000000001</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="1"/>
-        <v>5.3692927234404877</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="2"/>
-        <v>0.19900277777777778</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>126</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
-      <c r="H35" s="1">
-        <v>24.922999999999998</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="1"/>
+      <c r="E35" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L35">
-        <f t="shared" si="2"/>
-        <v>0.19780158730158728</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>51</v>
       </c>
@@ -1236,25 +893,14 @@
         <f t="shared" si="0"/>
         <v>1.0341392156862745</v>
       </c>
-      <c r="H36" s="1">
-        <v>9.92666</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="1"/>
-        <v>5.313076100118268</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="2"/>
-        <v>0.19464039215686274</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1266,69 +912,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4">
-        <f>AVERAGE(E4:E7,E9:E11,E13:E17,E19,E21:E34,E36)</f>
-        <v>1.0359268268929409</v>
+        <f>AVERAGE(E4:E36)</f>
+        <v>0.87896821675764691</v>
       </c>
       <c r="F39">
         <f>_xlfn.STDEV.P(E4:E36)</f>
-        <v>1.7060829738484645E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.37176417224093994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1422,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'revert-c7724c65' into 'master'"
This reverts merge request !1
</commit_message>
<xml_diff>
--- a/data_pi/bcode/perf_data_backup/runtime_results_for_graph.xlsx
+++ b/data_pi/bcode/perf_data_backup/runtime_results_for_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>average</t>
   </si>
@@ -54,13 +54,16 @@
   <si>
     <t>clock ticks in seconds</t>
   </si>
+  <si>
+    <t>PC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -129,7 +132,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,12 +428,12 @@
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -440,9 +443,12 @@
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>24</v>
       </c>
@@ -455,8 +461,11 @@
         <f>C4/A4</f>
         <v>1.0096375</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="1">
+        <v>4.4687700000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>18</v>
       </c>
@@ -469,8 +478,11 @@
         <f t="shared" ref="E5:E36" si="0">C5/A5</f>
         <v>1.052861111111111</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="1">
+        <v>3.5154000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>69</v>
       </c>
@@ -483,8 +495,11 @@
         <f t="shared" si="0"/>
         <v>1.0305623188405797</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="1">
+        <v>13.2567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36</v>
       </c>
@@ -497,8 +512,11 @@
         <f t="shared" si="0"/>
         <v>1.0061388888888887</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <v>6.8480299999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>15</v>
       </c>
@@ -509,8 +527,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="1">
+        <v>2.88348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>24</v>
       </c>
@@ -523,8 +544,11 @@
         <f t="shared" si="0"/>
         <v>1.0464374999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="1">
+        <v>4.74308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>21</v>
       </c>
@@ -537,8 +561,11 @@
         <f t="shared" si="0"/>
         <v>1.0145333333333333</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="1">
+        <v>4.0417399999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>27</v>
       </c>
@@ -551,8 +578,11 @@
         <f t="shared" si="0"/>
         <v>1.0504888888888888</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="1">
+        <v>5.33439</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>258</v>
       </c>
@@ -563,8 +593,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="1">
+        <v>49.197899999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>114</v>
       </c>
@@ -577,8 +610,11 @@
         <f t="shared" si="0"/>
         <v>1.0503157894736843</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="1">
+        <v>22.186599999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -591,8 +627,11 @@
         <f t="shared" si="0"/>
         <v>1.0379761904761904</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="1">
+        <v>8.2570800000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>57</v>
       </c>
@@ -605,8 +644,11 @@
         <f t="shared" si="0"/>
         <v>1.0612368421052631</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="1">
+        <v>11.2111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>24</v>
       </c>
@@ -619,8 +661,11 @@
         <f t="shared" si="0"/>
         <v>1.0368416666666667</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="1">
+        <v>4.5270299999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>27</v>
       </c>
@@ -633,8 +678,11 @@
         <f t="shared" si="0"/>
         <v>1.0145629629629629</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="1">
+        <v>5.11944</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -645,8 +693,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="1">
+        <v>2.9321799999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45</v>
       </c>
@@ -659,8 +710,11 @@
         <f t="shared" si="0"/>
         <v>1.0434177777777778</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="1">
+        <v>8.7858900000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -671,8 +725,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="1">
+        <v>2.8101799999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -685,8 +742,11 @@
         <f t="shared" si="0"/>
         <v>1.0174476190476189</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="1">
+        <v>3.9437799999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>27</v>
       </c>
@@ -699,8 +759,11 @@
         <f t="shared" si="0"/>
         <v>1.0475925925925926</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="1">
+        <v>5.3283800000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>51</v>
       </c>
@@ -713,8 +776,11 @@
         <f t="shared" si="0"/>
         <v>1.0536392156862744</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="1">
+        <v>10.084899999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>84</v>
       </c>
@@ -727,8 +793,11 @@
         <f t="shared" si="0"/>
         <v>1.0331785714285715</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="1">
+        <v>16.335599999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>27</v>
       </c>
@@ -741,8 +810,11 @@
         <f t="shared" si="0"/>
         <v>1.0538888888888889</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="1">
+        <v>5.2711100000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45</v>
       </c>
@@ -755,8 +827,11 @@
         <f t="shared" si="0"/>
         <v>1.0544755555555556</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="1">
+        <v>8.8572799999999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>36</v>
       </c>
@@ -769,8 +844,11 @@
         <f t="shared" si="0"/>
         <v>1.0373138888888889</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="1">
+        <v>6.9883199999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>39</v>
       </c>
@@ -783,8 +861,11 @@
         <f t="shared" si="0"/>
         <v>1.0201461538461538</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="1">
+        <v>7.6944999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>33</v>
       </c>
@@ -797,8 +878,11 @@
         <f t="shared" si="0"/>
         <v>1.0116424242424242</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H29" s="1">
+        <v>6.2503099999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -811,8 +895,11 @@
         <f t="shared" si="0"/>
         <v>1.0222074074074075</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="1">
+        <v>5.1136799999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>72</v>
       </c>
@@ -825,8 +912,11 @@
         <f t="shared" si="0"/>
         <v>1.0457444444444444</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="1">
+        <v>14.0959</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>72</v>
       </c>
@@ -839,8 +929,11 @@
         <f t="shared" si="0"/>
         <v>1.0364250000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="1">
+        <v>13.969900000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>21</v>
       </c>
@@ -853,8 +946,11 @@
         <f t="shared" si="0"/>
         <v>1.0145952380952381</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="1">
+        <v>4.0094099999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>72</v>
       </c>
@@ -867,8 +963,11 @@
         <f t="shared" si="0"/>
         <v>1.0685041666666666</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H34" s="1">
+        <v>14.328200000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>126</v>
       </c>
@@ -879,8 +978,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H35" s="1">
+        <v>24.922999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>51</v>
       </c>
@@ -893,14 +995,17 @@
         <f t="shared" si="0"/>
         <v>1.0341392156862745</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H36" s="1">
+        <v>9.92666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -912,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -926,55 +1031,55 @@
         <v>0.37176417224093994</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1068,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>